<commit_message>
member - feat performance bonus
</commit_message>
<xml_diff>
--- a/public/ClarkWell_Withdrawal_Import_Template.xlsx
+++ b/public/ClarkWell_Withdrawal_Import_Template.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Current Tech\Clarkwell v2\public\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\PhpstormProjects\clarkwellcrmv2\public\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{371933FD-901A-4DAE-A86D-3E33D89C861B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EBF81F1-0AF4-4553-AAD8-0218C27941D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{F9685B6B-FE6D-46A6-B998-C364933976CC}"/>
+    <workbookView xWindow="2250" yWindow="2250" windowWidth="21600" windowHeight="11835" xr2:uid="{F9685B6B-FE6D-46A6-B998-C364933976CC}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -47,9 +47,6 @@
     <t>amount</t>
   </si>
   <si>
-    <t>network</t>
-  </si>
-  <si>
     <t>status</t>
   </si>
   <si>
@@ -65,6 +62,9 @@
     <t>1 (pending), 
 2(approved), 
 3 (rejected)</t>
+  </si>
+  <si>
+    <t>method</t>
   </si>
 </sst>
 </file>
@@ -433,19 +433,19 @@
   <dimension ref="A1:E2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.77734375" customWidth="1"/>
-    <col min="2" max="2" width="7.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="35.6640625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" customWidth="1"/>
+    <col min="2" max="2" width="7.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="35.7109375" customWidth="1"/>
     <col min="4" max="4" width="21" customWidth="1"/>
     <col min="5" max="5" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -456,27 +456,27 @@
         <v>1</v>
       </c>
       <c r="D1" t="s">
+        <v>8</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+    </row>
+    <row r="2" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
         <v>4</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" ht="43.2" x14ac:dyDescent="0.3">
-      <c r="A2" s="1" t="s">
-        <v>5</v>
       </c>
       <c r="B2">
         <v>200</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>6</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" s="2" t="s">
         <v>7</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>